<commit_message>
Added IP field to db with new accesor methods
</commit_message>
<xml_diff>
--- a/database/data/user_data.xlsx
+++ b/database/data/user_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uctcloud-my.sharepoint.com/personal/ljndan001_myuct_ac_za/Documents/1- Courses/CSC3002F/Assignments/ass1/database/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="11_F25DC773A252ABDACC104877F15E584A5ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C4D916F5-262C-45BB-8DC9-BCF30AAFE805}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="11_F25DC773A252ABDACC104877F15E584A5ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3CB38254-C107-4306-8FCD-109A857CA1CD}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="2304" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>user_id</t>
   </si>
@@ -119,6 +119,78 @@
   </si>
   <si>
     <t>Burns</t>
+  </si>
+  <si>
+    <t>ip_address</t>
+  </si>
+  <si>
+    <t>88.60.241.111</t>
+  </si>
+  <si>
+    <t>2.157.164.237</t>
+  </si>
+  <si>
+    <t>181.87.13.187</t>
+  </si>
+  <si>
+    <t>187.160.100.85</t>
+  </si>
+  <si>
+    <t>62.182.139.127</t>
+  </si>
+  <si>
+    <t>27.158.255.22</t>
+  </si>
+  <si>
+    <t>117.105.21.50</t>
+  </si>
+  <si>
+    <t>8.248.52.152</t>
+  </si>
+  <si>
+    <t>7.190.48.73</t>
+  </si>
+  <si>
+    <t>153.53.191.20</t>
+  </si>
+  <si>
+    <t>24.29.158.165</t>
+  </si>
+  <si>
+    <t>21.184.96.247</t>
+  </si>
+  <si>
+    <t>DERPEN002</t>
+  </si>
+  <si>
+    <t>RAYMEA005</t>
+  </si>
+  <si>
+    <t>KELBON006</t>
+  </si>
+  <si>
+    <t>INDLAM001</t>
+  </si>
+  <si>
+    <t>EDIROM005</t>
+  </si>
+  <si>
+    <t>JAVBLA001</t>
+  </si>
+  <si>
+    <t>QUIHOU009</t>
+  </si>
+  <si>
+    <t>ALVTUC007</t>
+  </si>
+  <si>
+    <t>PHIPAL006</t>
+  </si>
+  <si>
+    <t>ALICHA008</t>
+  </si>
+  <si>
+    <t>JAVBUR009</t>
   </si>
 </sst>
 </file>
@@ -436,15 +508,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -454,8 +526,11 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -465,11 +540,13 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="str">
-        <f ca="1">UPPER(_xlfn.CONCAT(LEFT(B3,3),LEFT(C3, 3),"00",RANDBETWEEN(0, 9)))</f>
-        <v>DERPEN004</v>
+      <c r="D2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>41</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
@@ -477,11 +554,13 @@
       <c r="C3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="str">
-        <f t="shared" ref="A4:A13" ca="1" si="0">UPPER(_xlfn.CONCAT(LEFT(B4,3),LEFT(C4, 3),"00",RANDBETWEEN(0, 9)))</f>
-        <v>RAYMEA003</v>
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>42</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
@@ -489,11 +568,13 @@
       <c r="C4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>KELBON004</v>
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>43</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -501,11 +582,13 @@
       <c r="C5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>INDLAM001</v>
+      <c r="D5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>44</v>
       </c>
       <c r="B6" t="s">
         <v>12</v>
@@ -513,11 +596,13 @@
       <c r="C6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>EDIROM008</v>
+      <c r="D6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>45</v>
       </c>
       <c r="B7" t="s">
         <v>14</v>
@@ -525,11 +610,13 @@
       <c r="C7" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>JAVBLA009</v>
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>46</v>
       </c>
       <c r="B8" t="s">
         <v>16</v>
@@ -537,11 +624,13 @@
       <c r="C8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>QUIHOU006</v>
+      <c r="D8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>47</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
@@ -549,11 +638,13 @@
       <c r="C9" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>ALVTUC003</v>
+      <c r="D9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>48</v>
       </c>
       <c r="B10" t="s">
         <v>20</v>
@@ -561,11 +652,13 @@
       <c r="C10" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>PHIPAL001</v>
+      <c r="D10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>49</v>
       </c>
       <c r="B11" t="s">
         <v>22</v>
@@ -573,11 +666,13 @@
       <c r="C11" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>ALICHA008</v>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>50</v>
       </c>
       <c r="B12" t="s">
         <v>24</v>
@@ -585,17 +680,22 @@
       <c r="C12" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v>JAVBUR004</v>
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>51</v>
       </c>
       <c r="B13" t="s">
         <v>26</v>
       </c>
       <c r="C13" t="s">
         <v>27</v>
+      </c>
+      <c r="D13" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>